<commit_message>
Day1 - Done test case "FourOfAKind_88885_88885_Tie", "FourOfAKind_88885_88885_DifferentSuit_Tie", "FourOfAKind_88885_44442_FirstWin_KeyCard_8"
</commit_message>
<xml_diff>
--- a/src/PokerHands/Doc/Test cases.xlsx
+++ b/src/PokerHands/Doc/Test cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="278">
   <si>
     <t>Test case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1005,39 +1005,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FourOfAKind_88885_88885_Tie</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>8D,8C,8H,8S,5D</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8D,8C,8H,8S,5D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FourOfAKind_88885_88885_DifferentSuit_Tie</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>8D,8C,8H,8S,5C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FourOfAKind_44442_88885_SecondWin_KeyCard_8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4D,4S,2D,4H,4C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8D,8C,8H,8S,5C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Joe wins. - with four of a kind, key card 8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1129,6 +1105,38 @@
   </si>
   <si>
     <t>Joe wins. - with straight flush, key card 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FourOfAKind_88885_88885_Tie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8D,8C,8H,8S,5D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FourOfAKind_88885_88885_DifferentSuit_Tie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8D,8C,8H,8S,5D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4D,4S,2D,4H,4C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FourOfAKind_88885_44442_FirstWin_KeyCard_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tom wins. - with four of a kind, key card 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8D,8C,8H,8S,5C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1210,9 +1218,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1230,6 +1235,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1542,19 +1550,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="5"/>
+    <col min="1" max="1" width="9" style="4"/>
     <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.375" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.25" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1568,1294 +1576,1298 @@
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4"/>
+      <c r="G1" s="3"/>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="7">
+        <v>88885</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="7">
+        <v>88885</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" s="7">
+        <v>88885</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E2" s="8">
+      <c r="G3" s="7">
         <v>88885</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H3" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="7">
+        <v>88885</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G4" s="7">
+        <v>44442</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="G2" s="8">
-        <v>88885</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E3" s="8">
-        <v>88885</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E5" s="7">
+        <v>44442</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="G3" s="8">
-        <v>88885</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="6" t="s">
+      <c r="G5" s="7">
+        <v>44449</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E4" s="8">
-        <v>44442</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="G4" s="8">
-        <v>88885</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E5" s="8">
-        <v>44442</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="G5" s="8">
-        <v>44449</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>255</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>34567</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>55557</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>44422</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>44425</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>55667</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>65</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>34567</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F17" s="7"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>76</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>78</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>84</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="5" t="s">
         <v>88</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>100</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="5" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>108</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>110</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="9"/>
+      <c r="C26" s="5" t="s">
         <v>114</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>112</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="7" t="s">
         <v>118</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="5" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H29" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="5" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>135</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>137</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>139</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>141</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="7">
         <v>55883</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H34" s="5" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>157</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="H35" s="5" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="7">
         <v>33377</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="7">
         <v>33377</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="7">
         <v>33377</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="7">
         <v>33377</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="H37" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>166</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="7">
         <v>44425</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="H38" s="5" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="10"/>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="7" t="s">
         <v>168</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="7">
         <v>33324</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="H39" s="5" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="10"/>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="7" t="s">
         <v>174</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="8" t="s">
+      <c r="G40" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="H40" s="5" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="G41" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="H41" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="10"/>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="7" t="s">
         <v>179</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="H42" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="10"/>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="7" t="s">
         <v>39</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G43" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="H43" s="5" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="10"/>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="7" t="s">
         <v>188</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="7">
         <v>45678</v>
       </c>
-      <c r="H44" s="6" t="s">
+      <c r="H44" s="5" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="10"/>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>190</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="7">
         <v>45678</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="H45" s="5" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>193</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="7" t="s">
         <v>65</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="G46" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="H46" s="6" t="s">
+      <c r="H46" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>197</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="7" t="s">
         <v>196</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G47" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H47" s="6" t="s">
+      <c r="H47" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>199</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F48" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G48" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="H48" s="6" t="s">
+      <c r="H48" s="5" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="10"/>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="7" t="s">
         <v>207</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="G49" s="8" t="s">
+      <c r="G49" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="H49" s="6" t="s">
+      <c r="H49" s="5" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="10"/>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="5" t="s">
         <v>210</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G50" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="H50" s="6" t="s">
+      <c r="H50" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="10"/>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E51" s="7" t="s">
         <v>217</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="G51" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="H51" s="6" t="s">
+      <c r="H51" s="5" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="10"/>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="5" t="s">
         <v>220</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="F52" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="H52" s="6" t="s">
+      <c r="H52" s="5" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="5" t="s">
         <v>226</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="7" t="s">
         <v>228</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="G53" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="H53" s="6" t="s">
+      <c r="H53" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="10"/>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>229</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="7" t="s">
         <v>231</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="G54" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="H54" s="6" t="s">
+      <c r="H54" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="10"/>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="5" t="s">
         <v>233</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="F55" s="7" t="s">
+      <c r="F55" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="G55" s="8">
+      <c r="G55" s="7">
         <v>88822</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="H55" s="5" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="10"/>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="7" t="s">
         <v>240</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="7">
         <v>77744</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="H56" s="5" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>257</v>
+      <c r="B57" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>251</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>259</v>
+        <v>252</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>253</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="H57" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="H57" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="10"/>
-      <c r="C58" s="6" t="s">
-        <v>260</v>
+      <c r="C58" s="5" t="s">
+        <v>254</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>259</v>
+        <v>252</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>253</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="H58" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="H58" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
-      <c r="C59" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>264</v>
+      <c r="C59" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>258</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G59" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>267</v>
+        <v>259</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="10"/>
-      <c r="C60" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="E60" s="8" t="s">
+      <c r="C60" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="G60" s="8">
+      <c r="G60" s="7">
         <v>45678</v>
       </c>
-      <c r="H60" s="6" t="s">
-        <v>271</v>
+      <c r="H60" s="5" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
-      <c r="C61" s="6" t="s">
-        <v>272</v>
+      <c r="C61" s="5" t="s">
+        <v>266</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="G61" s="8">
+        <v>267</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G61" s="7">
         <v>45678</v>
       </c>
-      <c r="H61" s="6" t="s">
-        <v>275</v>
+      <c r="H61" s="5" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="B25:B30"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B57:B61"/>
     <mergeCell ref="B31:B35"/>
@@ -2863,9 +2875,6 @@
     <mergeCell ref="B41:B45"/>
     <mergeCell ref="B46:B52"/>
     <mergeCell ref="B53:B56"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="B25:B30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Day3(@Debbie) - Add pass test case
S05_FourOfAKind_FullHouse_FirstWin
S06_FullHouse_777JJ_88822_SecondWin_KeyCard_8
S07_FullHouse_777JJ_77744_FirstWin_KeyCard_Jack
</commit_message>
<xml_diff>
--- a/src/PokerHands/Doc/Test cases.xlsx
+++ b/src/PokerHands/Doc/Test cases.xlsx
@@ -92,22 +92,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FourOfAKind_FullHouse_FirstWin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5S,5D,5C,7S,5H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KD,8D,8S,8H,KS</t>
-  </si>
-  <si>
     <t>888KK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tom wins. - with four of a kind</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -117,10 +102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Flush_FullHouse_SecondWin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>8S,4S,TS,KS,AS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -959,39 +940,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FullHouse_777JJ_88822_SecondWin_KeyCard_8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AC,7S,7D,7H,AS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>777JJ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8D,8C,8H,2S,2D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Joe wins. - with full house, key card 8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FullHouse_777JJ_77744_FirstWin_KeyCard_Jack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AC,7S,7D,7H,AS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>777JJ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7D,7H,4D,4S,7S</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1137,6 +1090,54 @@
   </si>
   <si>
     <t>8D,8C,8H,8S,5C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FourOfAKind_FullHouse_FirstWin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5S,5D,5C,7S,5H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KD,8D,8S,8H,KS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tom wins. - with four of a kind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flush_FullHouse_SecondWin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FullHouse_777JJ_88822_SecondWin_KeyCard_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC,7S,7D,7H,AS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8D,8C,8H,2S,2D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Joe wins. - with full house, key card 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FullHouse_777JJ_77744_FirstWin_KeyCard_Jack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7D,7H,4D,4S,7S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JC,7S,7D,7H,JS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1144,7 +1145,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1189,6 +1190,20 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1210,7 +1225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1240,6 +1255,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1550,7 +1574,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1593,25 +1617,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="E2" s="7">
         <v>88885</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="G2" s="7">
         <v>88885</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1620,22 +1644,22 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="5" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="E3" s="7">
         <v>88885</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="G3" s="7">
         <v>88885</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1644,22 +1668,22 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="5" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="E4" s="7">
         <v>88885</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="G4" s="7">
         <v>44442</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1668,1213 +1692,1222 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="5" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="E5" s="7">
         <v>44442</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="G5" s="7">
         <v>44449</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="7"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="7">
-        <v>34567</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="E6" s="7">
+        <v>55557</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="7">
-        <v>55557</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="H6" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10"/>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>271</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>272</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>27</v>
+        <v>228</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>28</v>
+        <v>273</v>
       </c>
       <c r="G9" s="7">
-        <v>44422</v>
+        <v>88822</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
+      <c r="B10" s="10"/>
       <c r="C10" s="5" t="s">
-        <v>31</v>
+        <v>275</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>32</v>
+        <v>277</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>33</v>
+        <v>229</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>35</v>
+        <v>276</v>
+      </c>
+      <c r="G10" s="7">
+        <v>77744</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="7">
-        <v>44425</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="7"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>45</v>
+        <v>14</v>
+      </c>
+      <c r="E12" s="7">
+        <v>34567</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>50</v>
+        <v>270</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="G13" s="7">
-        <v>55667</v>
+        <v>44422</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>26</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>59</v>
+        <v>28</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>65</v>
+        <v>35</v>
+      </c>
+      <c r="G15" s="7">
+        <v>44425</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="7">
+        <v>55667</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="7">
+        <v>34567</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="E22" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="7">
-        <v>34567</v>
-      </c>
-      <c r="H16" s="5" t="s">
+      <c r="F22" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+      <c r="G22" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
-      <c r="C19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>99</v>
+        <v>75</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>96</v>
+        <v>73</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="5" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
-        <v>107</v>
-      </c>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
       <c r="C25" s="5" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>111</v>
+        <v>79</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="5" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>111</v>
+        <v>90</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
       <c r="C27" s="5" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
       <c r="C28" s="5" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>122</v>
+        <v>95</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="C29" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>126</v>
+        <v>103</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>122</v>
+        <v>105</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
       <c r="C30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="C31" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+      <c r="C32" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="C33" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F30" s="6" t="s">
+      <c r="D35" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="F35" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="9" t="s">
+      <c r="G35" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+      <c r="C36" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="D36" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E36" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F36" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G36" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
-      <c r="C32" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
-      <c r="C33" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" s="7">
-        <v>55883</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
-      <c r="C34" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-      <c r="C35" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E36" s="7">
-        <v>33377</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G36" s="7">
-        <v>33377</v>
-      </c>
       <c r="H36" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
       <c r="C37" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E37" s="7">
-        <v>33377</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>165</v>
+        <v>139</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="G37" s="7">
-        <v>33377</v>
+        <v>55883</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
       <c r="C38" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>167</v>
+        <v>144</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G38" s="7">
-        <v>44425</v>
+        <v>147</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>148</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="10"/>
       <c r="C39" s="5" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>2</v>
+        <v>151</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" s="7">
-        <v>33324</v>
+        <v>153</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>148</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="10"/>
+      <c r="B40" s="9" t="s">
+        <v>155</v>
+      </c>
       <c r="C40" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" s="7">
+        <v>33377</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G40" s="7">
+        <v>33377</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>175</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="9" t="s">
-        <v>176</v>
-      </c>
+      <c r="B41" s="10"/>
       <c r="C41" s="5" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>179</v>
+        <v>157</v>
+      </c>
+      <c r="E41" s="7">
+        <v>33377</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>181</v>
+        <v>160</v>
+      </c>
+      <c r="G41" s="7">
+        <v>33377</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="10"/>
       <c r="C42" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>178</v>
+        <v>161</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>179</v>
+        <v>163</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G42" s="7">
+        <v>44425</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>113</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="10"/>
       <c r="C43" s="5" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>185</v>
+        <v>3</v>
+      </c>
+      <c r="G43" s="7">
+        <v>33324</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="10"/>
       <c r="C44" s="5" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="7">
-        <v>45678</v>
+        <v>2</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="10"/>
+      <c r="B45" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="C45" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>6</v>
+        <v>172</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G45" s="7">
-        <v>45678</v>
+        <v>174</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>191</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="s">
-        <v>192</v>
-      </c>
+      <c r="B46" s="10"/>
       <c r="C46" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>194</v>
+        <v>177</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>65</v>
+        <v>174</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
       <c r="C47" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>198</v>
+        <v>179</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>196</v>
+        <v>34</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>195</v>
+        <v>6</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>113</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
       <c r="C48" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>200</v>
+        <v>182</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>203</v>
+        <v>183</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="7">
+        <v>45678</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="10"/>
       <c r="C49" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>206</v>
+        <v>185</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>203</v>
+        <v>180</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="7">
+        <v>45678</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="10"/>
+      <c r="B50" s="9" t="s">
+        <v>187</v>
+      </c>
       <c r="C50" s="5" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>212</v>
+        <v>60</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>214</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="10"/>
       <c r="C51" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>216</v>
+        <v>192</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>218</v>
+        <v>60</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>219</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="10"/>
       <c r="C52" s="5" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="9" t="s">
-        <v>225</v>
-      </c>
+      <c r="B53" s="10"/>
       <c r="C53" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>227</v>
+        <v>200</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>113</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="10"/>
       <c r="C54" s="5" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>227</v>
+        <v>202</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>113</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="10"/>
       <c r="C55" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>234</v>
+        <v>210</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>211</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="G55" s="7">
-        <v>88822</v>
+        <v>212</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>213</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="10"/>
       <c r="C56" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>239</v>
+        <v>215</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G56" s="7">
-        <v>77744</v>
+        <v>212</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>218</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="10"/>
       <c r="C58" s="5" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
       <c r="C59" s="5" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="10"/>
       <c r="C60" s="5" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="G60" s="7">
         <v>45678</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
       <c r="C61" s="5" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="G61" s="7">
         <v>45678</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="B29:B34"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B57:B61"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="B45:B49"/>
+    <mergeCell ref="B50:B56"/>
+    <mergeCell ref="B7:B10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Day4(@SK) - Add pass test csae
S08_FullHouse_ThreeOfAKind_SecondWin
S09_ThreeOfAKind_3332A_44425_SecondWin_KeyCard_4
S10_ThreeOfAKind_3332A_33324_FirstWin_KeyCard_Ace
S11_ThreeOfAKind_3335A_3332A_FirstWin_KeyCard_5
S12_ThreeOfAKind_TwoPairs_FirstWin
</commit_message>
<xml_diff>
--- a/src/PokerHands/Doc/Test cases.xlsx
+++ b/src/PokerHands/Doc/Test cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="284">
   <si>
     <t>Test case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -24,13 +24,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3C,3D,3H,AC,2S</t>
-  </si>
-  <si>
     <t>3C,3D,3H,2D,4S</t>
-  </si>
-  <si>
-    <t>3C,3D,3H,AC,5S</t>
   </si>
   <si>
     <t>TD,JS,QH,KD,AS</t>
@@ -194,10 +188,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Tom wins. - with three of a kind</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Two Pairs 
 vs 
 Pair</t>
@@ -646,34 +636,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ThreeOfAKind_33377_33377_Tie</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3D,7D,3S,7C,3C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3D,7D,3S,7C,3C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ThreeOfAKind_33377_33377_DifferentSuit_Tie</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3D,7H,3S,7S,3C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ThreeOfAKind_3332A_44425_SecondWin_KeyCard_4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3C,3D,3H,AC,2S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3332A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -686,23 +660,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ThreeOfAKind_3332A_33324_FirstWin_KeyCard_Acs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Tom wins. - with three of a kind, key card Ace</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ThreeOfAKind_3335A_3332A_FirstWin_KeyCard_5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3335A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tom wins. - with three of a kind, key card 5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1138,6 +1100,72 @@
   </si>
   <si>
     <t>JC,7S,7D,7H,JS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Full House 
+vs 
+Three of a Kind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Joe wins. - with full house</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FullHouse_ThreeOfAKind_SecondWin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4H,4S,4D,2C,5S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D,4S,2S,4D,4H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3C,3D,3H,AC,2S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3C,3D,3H,AC,2S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThreeOfAKind_3332A_33324_FirstWin_KeyCard_Ace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3C,3D,3H,AC,2S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThreeOfAKind_3335A_3332A_FirstWin_KeyCard_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3C,3D,3H,AC,5S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tom wins. - with three of a kind, key card 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tom wins. - with three of a kind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThreeOfAKind_33377_33377_Tie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D,7H,3S,7S,3C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1225,7 +1253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1264,6 +1292,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1570,7 +1604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1592,20 +1626,20 @@
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="1" t="s">
@@ -1616,98 +1650,98 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>231</v>
+      <c r="B2" s="14" t="s">
+        <v>221</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E2" s="7">
         <v>88885</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="G2" s="7">
         <v>88885</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="5" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="E3" s="7">
         <v>88885</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="G3" s="7">
         <v>88885</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="5" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="E4" s="7">
         <v>88885</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="G4" s="7">
         <v>44442</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="5" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="E5" s="7">
         <v>44442</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="G5" s="7">
         <v>44449</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1715,1198 +1749,1232 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="E6" s="7">
         <v>55557</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
-        <v>220</v>
+      <c r="B7" s="14" t="s">
+        <v>210</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="11" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="5" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="G9" s="7">
         <v>88822</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="5" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G10" s="7">
         <v>77744</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="7"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="E11" s="7">
+        <v>44425</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="G11" s="7">
+        <v>44422</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="13">
+        <v>33377</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="G12" s="13">
+        <v>33377</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="13">
+        <v>33377</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="G13" s="13">
+        <v>33377</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>9</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G14" s="7">
+        <v>44425</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>10</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="7">
+        <v>33324</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>11</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>12</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="7">
+        <v>34567</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="G18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="7">
+      <c r="H18" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="7">
+        <v>44422</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="7">
+        <v>44425</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="7">
+        <v>55667</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="7">
         <v>34567</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="7">
-        <v>44422</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="H26" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="14"/>
+      <c r="C29" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="14"/>
+      <c r="C30" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
+      <c r="C31" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="14"/>
+      <c r="C32" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="14"/>
+      <c r="C33" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="14"/>
+      <c r="C34" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="14"/>
+      <c r="C36" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="14"/>
+      <c r="C37" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="14"/>
+      <c r="C38" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="14"/>
+      <c r="C39" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="14"/>
+      <c r="C40" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="15"/>
+      <c r="C42" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="15"/>
+      <c r="C43" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G43" s="7">
+        <v>55883</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="15"/>
+      <c r="C44" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="15"/>
+      <c r="C45" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="15"/>
+      <c r="C47" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="15"/>
+      <c r="C48" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="F48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="15"/>
+      <c r="C49" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="7">
-        <v>44425</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="7">
-        <v>55667</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="7">
-        <v>34567</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-      <c r="C28" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
-      <c r="C30" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
-      <c r="C32" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="C33" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
-      <c r="C36" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-      <c r="C37" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G37" s="7">
-        <v>55883</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
-      <c r="C38" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="10"/>
-      <c r="C39" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E40" s="7">
-        <v>33377</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G40" s="7">
-        <v>33377</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
-      <c r="C41" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E41" s="7">
-        <v>33377</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="G41" s="7">
-        <v>33377</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
-      <c r="C42" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G42" s="7">
-        <v>44425</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
-      <c r="C43" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G43" s="7">
-        <v>33324</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="10"/>
-      <c r="C44" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="10"/>
-      <c r="C46" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="10"/>
-      <c r="C47" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="10"/>
-      <c r="C48" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" s="7">
-        <v>45678</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="10"/>
-      <c r="C49" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="G49" s="7">
         <v>45678</v>
       </c>
       <c r="H49" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="15"/>
+      <c r="C50" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="7">
+        <v>45678</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="15"/>
+      <c r="C52" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="15"/>
+      <c r="C53" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E53" s="7" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="9" t="s">
+      <c r="F53" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="G53" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="H53" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="E50" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F50" s="1" t="s">
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="15"/>
+      <c r="C54" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="G50" s="7" t="s">
+      <c r="D54" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="H50" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="10"/>
-      <c r="C51" s="5" t="s">
+      <c r="E54" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E51" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="10"/>
-      <c r="C52" s="5" t="s">
+      <c r="G54" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="H54" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D52" s="1" t="s">
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="15"/>
+      <c r="C55" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="D55" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="E55" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="G52" s="7" t="s">
+      <c r="G55" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H55" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="10"/>
-      <c r="C53" s="5" t="s">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="15"/>
+      <c r="C56" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D56" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E56" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F56" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G56" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="G53" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="H53" s="5" t="s">
+      <c r="H56" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="10"/>
-      <c r="C54" s="5" t="s">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="15"/>
+      <c r="C57" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E57" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="F57" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="G54" s="7" t="s">
+      <c r="G57" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="H57" s="5" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="10"/>
-      <c r="C55" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="10"/>
-      <c r="C56" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="9" t="s">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="15"/>
+      <c r="C59" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="15"/>
+      <c r="C60" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="H60" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="D57" s="1" t="s">
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="15"/>
+      <c r="C61" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="D61" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="10"/>
-      <c r="C58" s="5" t="s">
+      <c r="E61" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="10"/>
-      <c r="C59" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="10"/>
-      <c r="C60" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="G60" s="7">
-        <v>45678</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="10"/>
-      <c r="C61" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="G61" s="7">
         <v>45678</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>257</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="15"/>
+      <c r="C62" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="G62" s="7">
+        <v>45678</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="B35:B40"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="B45:B49"/>
-    <mergeCell ref="B50:B56"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="B51:B57"/>
     <mergeCell ref="B7:B10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Day5(@Paul) - Add pass test case
S13_TwoPairs_22JJ5_55883_FirstWin_KeyCard_Jack
S14_TwoPairs_22JJ5_55JJ3_SecondWin_KeyCard_5
S15_TwoPairs_55JJA_55JJ3_FirstWin_KeyCard_Ace
S16_Straight_ThreeOfAKind_FirstWin
S17_Straight_TJQKA_A2345_FirstWin_KeyCard_King
</commit_message>
<xml_diff>
--- a/src/PokerHands/Doc/Test cases.xlsx
+++ b/src/PokerHands/Doc/Test cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="288">
   <si>
     <t>Test case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -148,15 +148,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Straight_ThreeOfAKind_FirstWin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TJQKA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4H,4S,4D,2C,5S</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -559,22 +551,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5S,JH,6D,6H,5C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5566J</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TwoPairs_22JJ5_55883_FirstWin_KeyCard_Jack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5C,JS,JH,2S,2C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>22JJ5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -583,26 +563,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Tom wins. - with two pairs, key card Jack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TwoPairs_22JJ5_55JJ3_SecondWin_KeyCard_5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5C,JS,JH,2S,2C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>22JJ5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5C,JD,JS,5D,3H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>55JJ3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -611,22 +575,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TwoPairs_55JJA_55JJ3_FirstWin_KeyCard_Acs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5D,5S,AD,JS,JD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>55JJA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5C,JD,JS,5D,3H</t>
-  </si>
-  <si>
-    <t>Tom wins. - with two pairs, key card Acs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -686,14 +635,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7S,8D,9S,TC,JS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>789TJ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Straight_789TJ_789TJ_DifferentSuit_Tie</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -710,19 +651,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Tom wins. - with straight, key card King</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Straight_TJQKA_45678_FirstWin_KeyCard_Acs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TJQKA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tom wins. - with straight, key card Acs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -764,10 +693,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Flush_2589Q_35TJA_SecondWin_KeyCard_Acs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5C,8C,9C,2C,QC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -781,10 +706,6 @@
   </si>
   <si>
     <t>35TJA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Joe wins. - with flush, key card Acs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -991,19 +912,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>StraightFlush_TJQKA_45678_FirstWin_KeyCard_Acs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TS,JS,QS,KS,AS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>8C,6C,4C,5C,7C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tom wins. - with straight flush, key card Acs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1166,6 +1079,104 @@
   </si>
   <si>
     <t>3D,7H,3S,7S,3C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TwoPairs_22JJ5_55883_FirstWin_KeyCard_Jack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5C,JS,JH,2S,2C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tom wins. - with two pairs, key card Jack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TwoPairs_22JJ5_55JJ3_SecondWin_KeyCard_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5C,JS,JH,2S,2C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5C,JD,JS,5D,3H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TwoPairs_55JJA_55JJ3_FirstWin_KeyCard_Ace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tom wins. - with two pairs, key card Ace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5D,5S,AD,JS,JD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5C,JD,JS,5D,3H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Straight_ThreeOfAKind_FirstWin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TD,JS,QH,KD,AS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4H,4S,4D,2C,5S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Straight_TJQKA_45678_FirstWin_KeyCard_Ace</t>
+  </si>
+  <si>
+    <t>Tom wins. - with straight, key card Ace</t>
+  </si>
+  <si>
+    <t>Flush_2589Q_35TJA_SecondWin_KeyCard_Ace</t>
+  </si>
+  <si>
+    <t>Joe wins. - with flush, key card Ace</t>
+  </si>
+  <si>
+    <t>StraightFlush_TJQKA_45678_FirstWin_KeyCard_Ace</t>
+  </si>
+  <si>
+    <t>Tom wins. - with straight flush, key card Ace</t>
+  </si>
+  <si>
+    <t>TD,JS,QH,KD,AS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D,5S,4C,3C,AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tom wins. - with straight, key card King</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5S,JH,6D,6H,5C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>789TJ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tie</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1253,7 +1264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1292,6 +1303,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1604,11 +1618,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1634,10 +1648,10 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="E1" s="15"/>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1650,98 +1664,98 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>221</v>
+      <c r="B2" s="15" t="s">
+        <v>201</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
       <c r="E2" s="7">
         <v>88885</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="G2" s="7">
         <v>88885</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="5" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="E3" s="7">
         <v>88885</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="G3" s="7">
         <v>88885</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="5" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="E4" s="7">
         <v>88885</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="G4" s="7">
         <v>44442</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="5" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="E5" s="7">
         <v>44442</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="G5" s="7">
         <v>44449</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1752,114 +1766,114 @@
         <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="E6" s="7">
         <v>55557</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>210</v>
+      <c r="B7" s="15" t="s">
+        <v>190</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="11" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="5" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="G9" s="7">
         <v>88822</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="5" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="G10" s="7">
         <v>77744</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -1867,108 +1881,108 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="E11" s="7">
         <v>44425</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="G11" s="7">
         <v>44422</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
-        <v>152</v>
+      <c r="B12" s="15" t="s">
+        <v>139</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E12" s="13">
         <v>33377</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="G12" s="13">
         <v>33377</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="11" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E13" s="13">
         <v>33377</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="G13" s="13">
         <v>33377</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>9</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="5" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="G14" s="7">
         <v>44425</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>10</v>
       </c>
-      <c r="B15" s="15"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="5" t="s">
-        <v>275</v>
+        <v>253</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>2</v>
@@ -1977,31 +1991,31 @@
         <v>33324</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>11</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="5" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>279</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2009,972 +2023,995 @@
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="E17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="F17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="16"/>
+      <c r="C19" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>13</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="7">
+        <v>55883</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>14</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>15</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>16</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G23" s="7">
+        <v>44425</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="16"/>
+      <c r="C25" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>17</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="16"/>
+      <c r="C27" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="7">
+        <v>45678</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="16"/>
+      <c r="C28" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="7">
+        <v>45678</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="7">
+        <v>34567</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="7">
+        <v>44422</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="C34" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="7">
+      <c r="D34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="7">
+        <v>55667</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="7">
         <v>34567</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="7">
-        <v>44422</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="7">
-        <v>44425</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" s="7">
-        <v>55667</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="H37" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" s="6" t="s">
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="7">
-        <v>34567</v>
-      </c>
-      <c r="H26" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
+      <c r="D39" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="E39" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="H39" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G28" s="7" t="s">
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="15"/>
+      <c r="C40" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="D40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="14"/>
-      <c r="C29" s="5" t="s">
+      <c r="G40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="15"/>
+      <c r="C41" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="D41" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="14"/>
-      <c r="C30" s="5" t="s">
+      <c r="E41" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="F41" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="H41" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="14"/>
-      <c r="C31" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="14"/>
-      <c r="C32" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="14"/>
-      <c r="C33" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="14"/>
-      <c r="C34" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="14"/>
-      <c r="C36" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="14"/>
-      <c r="C37" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="14"/>
-      <c r="C38" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="14"/>
-      <c r="C39" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="14"/>
-      <c r="C40" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="15"/>
       <c r="C42" s="5" t="s">
-        <v>131</v>
+        <v>78</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>134</v>
+        <v>74</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="15"/>
       <c r="C43" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>137</v>
+        <v>83</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G43" s="7">
-        <v>55883</v>
+        <v>85</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="15"/>
       <c r="C44" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>142</v>
+        <v>88</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>144</v>
+        <v>90</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="15"/>
       <c r="C45" s="5" t="s">
-        <v>147</v>
+        <v>92</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="14" t="s">
-        <v>161</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>163</v>
+        <v>98</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>165</v>
+        <v>100</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="15"/>
       <c r="C47" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>163</v>
+        <v>104</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>164</v>
+        <v>102</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>168</v>
+        <v>101</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="15"/>
       <c r="C48" s="5" t="s">
-        <v>169</v>
+        <v>106</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>170</v>
+        <v>102</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="15"/>
       <c r="C49" s="5" t="s">
-        <v>172</v>
+        <v>110</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G49" s="7">
-        <v>45678</v>
+        <v>111</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>174</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="15"/>
       <c r="C50" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="15"/>
+      <c r="C51" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="16"/>
+      <c r="C53" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="16"/>
+      <c r="C54" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="16"/>
+      <c r="C55" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="16"/>
+      <c r="C56" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G50" s="7">
-        <v>45678</v>
-      </c>
-      <c r="H50" s="5" t="s">
+      <c r="D56" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
+      <c r="E56" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F56" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="G56" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="H56" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="E51" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F51" s="1" t="s">
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="16"/>
+      <c r="C57" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="D57" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H51" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="15"/>
-      <c r="C52" s="5" t="s">
+      <c r="E57" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="F57" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G57" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="E52" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="15"/>
-      <c r="C53" s="5" t="s">
+      <c r="H57" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D53" s="1" t="s">
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="16"/>
+      <c r="C58" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="D58" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="E58" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F58" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="G58" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="H58" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="15"/>
-      <c r="C54" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="15"/>
-      <c r="C55" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="15"/>
-      <c r="C56" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="15"/>
-      <c r="C57" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="G57" s="7" t="s">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="C59" s="5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="15"/>
-      <c r="C59" s="5" t="s">
-        <v>232</v>
-      </c>
       <c r="D59" s="1" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="15"/>
+      <c r="B60" s="16"/>
       <c r="C60" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>235</v>
+        <v>212</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>238</v>
+        <v>211</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>239</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="15"/>
+      <c r="B61" s="16"/>
       <c r="C61" s="5" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G61" s="7">
-        <v>45678</v>
+        <v>217</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>218</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="15"/>
+      <c r="B62" s="16"/>
       <c r="C62" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>245</v>
+        <v>279</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>220</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>246</v>
+        <v>216</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="G62" s="7">
         <v>45678</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>247</v>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="16"/>
+      <c r="C63" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="G63" s="7">
+        <v>45678</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="B46:B51"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="B18:B22"/>
     <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="B51:B57"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B52:B58"/>
     <mergeCell ref="B7:B10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Day6(@KK) - Add pass test case
S18_Straight_TJQKA_45678_FirstWin_KeyCard_Ace
S19_Straight_A2345_45678_SecondWin_KeyCard_8
</commit_message>
<xml_diff>
--- a/src/PokerHands/Doc/Test cases.xlsx
+++ b/src/PokerHands/Doc/Test cases.xlsx
@@ -659,10 +659,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Tom wins. - with straight, key card 8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Flush 
 vs 
 Flush</t>
@@ -1177,6 +1173,10 @@
   </si>
   <si>
     <t>Tie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Joe wins. - with straight, key card 8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1621,8 +1621,8 @@
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1665,19 +1665,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="E2" s="7">
         <v>88885</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G2" s="7">
         <v>88885</v>
@@ -1692,16 +1692,16 @@
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="E3" s="7">
         <v>88885</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G3" s="7">
         <v>88885</v>
@@ -1716,22 +1716,22 @@
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E4" s="7">
         <v>88885</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G4" s="7">
         <v>44442</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1740,22 +1740,22 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E5" s="7">
         <v>44442</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G5" s="7">
         <v>44449</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1766,42 +1766,42 @@
         <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>235</v>
       </c>
       <c r="E6" s="7">
         <v>55557</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>193</v>
-      </c>
       <c r="F7" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>192</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>193</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>103</v>
@@ -1810,19 +1810,19 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
       <c r="C8" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>196</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>197</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>103</v>
@@ -1834,22 +1834,22 @@
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>241</v>
       </c>
       <c r="G9" s="7">
         <v>88822</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1858,22 +1858,22 @@
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="G10" s="7">
         <v>77744</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -1881,25 +1881,25 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>248</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>249</v>
       </c>
       <c r="E11" s="7">
         <v>44425</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G11" s="7">
         <v>44422</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1907,7 +1907,7 @@
         <v>139</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>140</v>
@@ -1922,7 +1922,7 @@
         <v>33377</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1937,13 +1937,13 @@
         <v>33377</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G13" s="13">
         <v>33377</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1955,7 +1955,7 @@
         <v>142</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>143</v>
@@ -1976,10 +1976,10 @@
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>143</v>
@@ -2000,22 +2000,22 @@
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>147</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>143</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2041,7 +2041,7 @@
         <v>38</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2079,7 +2079,7 @@
         <v>131</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>132</v>
@@ -2094,10 +2094,10 @@
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>262</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>263</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>133</v>
@@ -2109,7 +2109,7 @@
         <v>55883</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2118,16 +2118,16 @@
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>266</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>135</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>136</v>
@@ -2142,22 +2142,22 @@
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>138</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>136</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2168,16 +2168,16 @@
         <v>30</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G23" s="7">
         <v>44425</v>
@@ -2203,10 +2203,10 @@
         <v>150</v>
       </c>
       <c r="G24" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>285</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
         <v>151</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2239,25 +2239,28 @@
         <v>154</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>155</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>18</v>
+      </c>
       <c r="B27" s="16"/>
       <c r="C27" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>3</v>
@@ -2272,10 +2275,13 @@
         <v>45678</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>19</v>
+      </c>
       <c r="B28" s="16"/>
       <c r="C28" s="5" t="s">
         <v>157</v>
@@ -2293,7 +2299,7 @@
         <v>45678</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>158</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2332,7 +2338,7 @@
         <v>18</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>19</v>
@@ -2747,22 +2753,22 @@
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="D52" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G52" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>69</v>
@@ -2771,16 +2777,16 @@
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="16"/>
       <c r="C53" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="E53" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>55</v>
@@ -2792,126 +2798,126 @@
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="16"/>
       <c r="C54" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="H54" s="5" t="s">
         <v>277</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="16"/>
       <c r="C55" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="E55" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="F55" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="H55" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="16"/>
       <c r="C56" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F56" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E56" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="F56" s="6" t="s">
+      <c r="G56" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="G56" s="7" t="s">
+      <c r="H56" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="16"/>
       <c r="C57" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="E57" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="F57" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G57" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G57" s="7" t="s">
+      <c r="H57" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="16"/>
       <c r="C58" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F58" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="E58" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="F58" s="6" t="s">
+      <c r="G58" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="G58" s="7" t="s">
+      <c r="H58" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="D59" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="E59" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="F59" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G59" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>69</v>
@@ -2920,19 +2926,19 @@
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="16"/>
       <c r="C60" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="G60" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>69</v>
@@ -2941,64 +2947,64 @@
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="16"/>
       <c r="C61" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="E61" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="F61" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="G61" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="G61" s="7" t="s">
+      <c r="H61" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="16"/>
       <c r="C62" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D62" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="G62" s="7">
         <v>45678</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="16"/>
       <c r="C63" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F63" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="G63" s="7">
         <v>45678</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day8(@IanLiang) - Add pass test case
S23_Pair_TwoPairs_SecondWin
S24_HighCard_Pair_SecondWin
S25_HighCard_3479K_248TK_SecondWin_KeyCard_Ten
S26_Flush_HighCard_SamePoint_FirstWin
S27_HighCard_367JA_367JA_Tie
S28_StraightFlush_FourOfAKind_FirstWin
S29_Flush_FullHouse_SecondWin
</commit_message>
<xml_diff>
--- a/src/PokerHands/Doc/Test cases.xlsx
+++ b/src/PokerHands/Doc/Test cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="289">
   <si>
     <t>Test case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,19 +64,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3D,5D,7D,4D,6D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AS,AH,AD,AC,KD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AAAAK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tom wins. - with straight flush</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -104,10 +92,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2D,4S,2S,4D,4H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Joe wins. - with full house</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -172,21 +156,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Pair_TwoPairs_SecondWin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5S,JH,6S,JC,AS</t>
-  </si>
-  <si>
     <t>JJ56A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5D,7D,6S,6C,5H</t>
-  </si>
-  <si>
-    <t>Joe wins. - with two pairs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -196,13 +166,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HighCard_Pair_SecondWin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JD,7D,KS,6S,3C</t>
-  </si>
-  <si>
     <t>367JK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -212,10 +175,6 @@
   </si>
   <si>
     <t>AA46K</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Joe wins. - with pair</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -225,19 +184,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Flush_HighCard_SamePoint_FirstWin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2C,6C,8C,4C,TC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2468T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TC,8D,4H,6S,2C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -251,10 +198,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HighCard_367JA_367JA_Tie</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>JD,7D,AS,6S,3C</t>
   </si>
   <si>
@@ -262,9 +205,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AS,JD,7D,3C,6S</t>
-  </si>
-  <si>
     <t>367JA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -304,13 +244,6 @@
   </si>
   <si>
     <t>HighCard_3479K_248TK_SecondWin_KeyCard_Ten</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KS,7D,3C,9H,4D</t>
-  </si>
-  <si>
-    <t>2D,4S,KD,TS,8S</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -929,10 +862,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Flush_FullHouse_SecondWin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FullHouse_777JJ_88822_SecondWin_KeyCard_8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1178,6 +1107,86 @@
   </si>
   <si>
     <t>Joe wins. - with straight flush</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pair_TwoPairs_SecondWin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5S,JH,6S,JC,AS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5D,7D,6S,6C,5H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Joe wins. - with two pairs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HighCard_Pair_SecondWin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JD,7D,KS,6S,3C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Joe wins. - with pair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KS,7D,3C,9H,4D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D,4S,KD,TS,8S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flush_HighCard_SamePoint_FirstWin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C,6C,8C,4C,TC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC,8D,4H,6S,2C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HighCard_367JA_367JA_Tie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JD,7D,AS,6S,3C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AS,JD,7D,3C,6S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D,5D,7D,4D,6D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AS,AH,AD,AC,KD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tom wins. - with straight flush</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flush_FullHouse_SecondWin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D,4S,2S,4D,4H</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1628,8 +1637,8 @@
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41:XFD41"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1672,25 +1681,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="E2" s="7">
         <v>88885</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="G2" s="7">
         <v>88885</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1699,22 +1708,22 @@
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="5" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="E3" s="7">
         <v>88885</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="G3" s="7">
         <v>88885</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1723,22 +1732,22 @@
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="5" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="E4" s="7">
         <v>88885</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="G4" s="7">
         <v>44442</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1747,22 +1756,22 @@
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="5" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="E5" s="7">
         <v>44442</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="G5" s="7">
         <v>44449</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1770,69 +1779,69 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="E6" s="7">
         <v>55557</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
       <c r="C8" s="11" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1841,22 +1850,22 @@
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="5" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="G9" s="7">
         <v>88822</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1865,22 +1874,22 @@
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="5" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="G10" s="7">
         <v>77744</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -1888,69 +1897,69 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="E11" s="7">
         <v>44425</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="G11" s="7">
         <v>44422</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="E12" s="13">
         <v>33377</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="G12" s="13">
         <v>33377</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="11" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="E13" s="13">
         <v>33377</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="G13" s="13">
         <v>33377</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1959,22 +1968,22 @@
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="5" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="G14" s="7">
         <v>44425</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1983,13 +1992,13 @@
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="5" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>2</v>
@@ -1998,7 +2007,7 @@
         <v>33324</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2007,22 +2016,22 @@
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="5" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2030,69 +2039,69 @@
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="G17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="H17" s="5" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
       <c r="C19" s="11" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2101,22 +2110,22 @@
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="5" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="G20" s="7">
         <v>55883</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2125,22 +2134,22 @@
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="5" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2149,22 +2158,22 @@
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="5" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2172,69 +2181,69 @@
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="G23" s="7">
         <v>44425</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="18"/>
       <c r="C25" s="11" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2243,22 +2252,22 @@
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="5" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2267,13 +2276,13 @@
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="5" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>5</v>
@@ -2282,7 +2291,7 @@
         <v>45678</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2291,13 +2300,13 @@
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="5" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>5</v>
@@ -2306,7 +2315,7 @@
         <v>45678</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2318,6 +2327,9 @@
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>28</v>
+      </c>
       <c r="B30" s="2" t="s">
         <v>10</v>
       </c>
@@ -2325,42 +2337,45 @@
         <v>11</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>12</v>
+        <v>284</v>
       </c>
       <c r="E30" s="7">
         <v>34567</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>13</v>
+        <v>285</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H30" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C31" s="5" t="s">
-        <v>225</v>
+        <v>287</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>21</v>
+        <v>288</v>
       </c>
       <c r="G31" s="7">
         <v>44422</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2368,94 +2383,103 @@
         <v>20</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>23</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>37</v>
+        <v>269</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>38</v>
+        <v>270</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>40</v>
+        <v>271</v>
       </c>
       <c r="G34" s="7">
         <v>55667</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>41</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>24</v>
+      </c>
       <c r="B35" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>43</v>
+        <v>273</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>44</v>
+        <v>274</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>48</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>26</v>
+      </c>
       <c r="B36" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>50</v>
+        <v>278</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>51</v>
+        <v>279</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>53</v>
+        <v>280</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2463,25 +2487,25 @@
         <v>22</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G37" s="7">
         <v>34567</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2494,345 +2518,351 @@
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>27</v>
+      </c>
       <c r="B39" s="17" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>56</v>
+        <v>281</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>57</v>
+        <v>282</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>59</v>
+        <v>283</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="17"/>
       <c r="C40" s="5" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="17"/>
       <c r="C41" s="5" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>25</v>
+      </c>
       <c r="B42" s="17"/>
       <c r="C42" s="5" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>71</v>
+        <v>276</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>72</v>
+        <v>277</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="17"/>
       <c r="C43" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" s="17"/>
       <c r="C44" s="5" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="17"/>
       <c r="C45" s="5" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="17" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="17"/>
       <c r="C47" s="5" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="17"/>
       <c r="C48" s="5" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" s="17"/>
       <c r="C49" s="5" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" s="17"/>
       <c r="C50" s="5" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" s="17"/>
       <c r="C51" s="5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="17" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" s="18"/>
       <c r="C53" s="5" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="18"/>
       <c r="C54" s="5" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2841,192 +2871,192 @@
       </c>
       <c r="B55" s="18"/>
       <c r="C55" s="5" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" s="18"/>
       <c r="C56" s="5" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" s="18"/>
       <c r="C57" s="5" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" s="18"/>
       <c r="C58" s="5" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B59" s="17" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" s="18"/>
       <c r="C60" s="5" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" s="18"/>
       <c r="C61" s="5" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" s="18"/>
       <c r="C62" s="5" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="G62" s="7">
         <v>45678</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B63" s="18"/>
       <c r="C63" s="5" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="G63" s="7">
         <v>45678</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add left all test case
</commit_message>
<xml_diff>
--- a/src/PokerHands/Doc/Test cases.xlsx
+++ b/src/PokerHands/Doc/Test cases.xlsx
@@ -403,10 +403,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>QC,QS,2D,5S,JS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>QQ35J</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -673,10 +669,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FullHouse_555QQ_555QQ_Tie</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5C,5H,5S,QD,QH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1187,6 +1179,14 @@
   </si>
   <si>
     <t>2D,4S,2S,4D,4H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FullHouse_555QQ_555QQ_Tie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QC,QS,3D,5S,JS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1274,7 +1274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1313,15 +1313,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1634,11 +1625,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1664,10 +1655,10 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1680,20 +1671,20 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>170</v>
+      <c r="B2" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E2" s="7">
         <v>88885</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G2" s="7">
         <v>88885</v>
@@ -1706,18 +1697,18 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E3" s="7">
         <v>88885</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G3" s="7">
         <v>88885</v>
@@ -1730,48 +1721,48 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="E4" s="7">
         <v>88885</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G4" s="7">
         <v>44442</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E5" s="7">
         <v>44442</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G5" s="7">
         <v>44449</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1782,63 +1773,69 @@
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E6" s="7">
         <v>55557</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="4">
+        <v>30</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="E7" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>162</v>
-      </c>
       <c r="F7" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
+      <c r="A8" s="4">
+        <v>31</v>
+      </c>
+      <c r="B8" s="15"/>
       <c r="C8" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="F8" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>164</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>166</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>77</v>
@@ -1848,48 +1845,48 @@
       <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>209</v>
       </c>
       <c r="G9" s="7">
         <v>88822</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>213</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G10" s="7">
         <v>77744</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -1897,108 +1894,114 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="D11" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E11" s="7">
         <v>44425</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G11" s="7">
         <v>44422</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="4">
+        <v>32</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>113</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>114</v>
       </c>
       <c r="E12" s="13">
         <v>33377</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G12" s="13">
         <v>33377</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
+      <c r="A13" s="4">
+        <v>33</v>
+      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E13" s="13">
         <v>33377</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G13" s="13">
         <v>33377</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>9</v>
       </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="G14" s="7">
         <v>44425</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>10</v>
       </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>2</v>
@@ -2007,31 +2010,31 @@
         <v>33324</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>11</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2057,48 +2060,54 @@
         <v>31</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="4">
+        <v>34</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="E18" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="G18" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
+      <c r="A19" s="4">
+        <v>35</v>
+      </c>
+      <c r="B19" s="15"/>
       <c r="C19" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>105</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>45</v>
@@ -2108,72 +2117,72 @@
       <c r="A20" s="4">
         <v>13</v>
       </c>
-      <c r="B20" s="18"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E20" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="G20" s="7">
         <v>55883</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>14</v>
       </c>
-      <c r="B21" s="18"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E21" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="G21" s="7" t="s">
+      <c r="H21" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>15</v>
       </c>
-      <c r="B22" s="18"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>238</v>
-      </c>
       <c r="E22" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2184,16 +2193,16 @@
         <v>23</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G23" s="7">
         <v>44425</v>
@@ -2203,86 +2212,92 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="4">
+        <v>36</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="E24" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="F24" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>37</v>
+      </c>
+      <c r="B25" s="15"/>
+      <c r="C25" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="D25" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="F25" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>253</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>17</v>
       </c>
-      <c r="B26" s="18"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>18</v>
       </c>
-      <c r="B27" s="18"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>5</v>
@@ -2291,22 +2306,22 @@
         <v>45678</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>19</v>
       </c>
-      <c r="B28" s="18"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>5</v>
@@ -2315,761 +2330,810 @@
         <v>45678</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="5"/>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E29" s="7">
+        <v>34567</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="E30" s="7">
-        <v>34567</v>
-      </c>
-      <c r="F30" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="G30" s="7" t="s">
-        <v>12</v>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="G30" s="7">
+        <v>44422</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>286</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>15</v>
+        <v>255</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>16</v>
+        <v>256</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="G31" s="7">
-        <v>44422</v>
+        <v>20</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>18</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>257</v>
+        <v>32</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>19</v>
+        <v>267</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>268</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G32" s="7">
+        <v>55667</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>259</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>24</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>270</v>
+        <v>276</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>277</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="G34" s="7">
-        <v>55667</v>
+        <v>39</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>272</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>34</v>
+        <v>262</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G35" s="7">
+        <v>34567</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>27</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>38</v>
+      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>39</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>25</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H35" s="5" t="s">
+      <c r="E39" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>26</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H36" s="5" t="s">
+      <c r="G39" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>22</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="G37" s="7">
-        <v>34567</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="5"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>27</v>
-      </c>
-      <c r="B39" s="17" t="s">
+      <c r="B40" s="14"/>
+      <c r="C40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
         <v>41</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="17"/>
-      <c r="C40" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="17"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="5" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>25</v>
-      </c>
-      <c r="B42" s="17"/>
+        <v>42</v>
+      </c>
+      <c r="B42" s="14"/>
       <c r="C42" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>276</v>
+        <v>66</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="E42" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>43</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>44</v>
+      </c>
+      <c r="B44" s="14"/>
+      <c r="C44" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>45</v>
+      </c>
+      <c r="B45" s="14"/>
+      <c r="C45" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>46</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>47</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>48</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>49</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
         <v>50</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="17"/>
-      <c r="C43" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="17"/>
-      <c r="C44" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="17"/>
-      <c r="C45" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="H46" s="5" t="s">
+      <c r="B50" s="15"/>
+      <c r="C50" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H50" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="17"/>
-      <c r="C47" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="17"/>
-      <c r="C48" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="17"/>
-      <c r="C49" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="17"/>
-      <c r="C50" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="17"/>
+      <c r="A51" s="4">
+        <v>51</v>
+      </c>
+      <c r="B51" s="15"/>
       <c r="C51" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>90</v>
+        <v>243</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>97</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="17" t="s">
-        <v>132</v>
-      </c>
+      <c r="A52" s="4">
+        <v>21</v>
+      </c>
+      <c r="B52" s="15"/>
       <c r="C52" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>134</v>
+        <v>258</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>135</v>
+        <v>260</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>45</v>
+        <v>261</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="18"/>
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="15"/>
       <c r="C53" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>39</v>
+        <v>146</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="18"/>
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" s="15"/>
       <c r="C54" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>139</v>
+        <v>148</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>141</v>
+        <v>150</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>246</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>21</v>
-      </c>
-      <c r="B55" s="18"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="15"/>
       <c r="C55" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>261</v>
+        <v>153</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>262</v>
+        <v>150</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>263</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="18"/>
+      <c r="A56" s="4">
+        <v>55</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>175</v>
+      </c>
       <c r="C56" s="5" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>146</v>
+        <v>178</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>148</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="18"/>
+      <c r="A57" s="4">
+        <v>56</v>
+      </c>
+      <c r="B57" s="15"/>
       <c r="C57" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>150</v>
+        <v>179</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>153</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="18"/>
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
+      <c r="B58" s="15"/>
       <c r="C58" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>155</v>
+        <v>181</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>156</v>
+        <v>183</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="17" t="s">
-        <v>177</v>
-      </c>
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="15"/>
       <c r="C59" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>179</v>
+        <v>245</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>180</v>
+        <v>188</v>
+      </c>
+      <c r="G59" s="7">
+        <v>45678</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>45</v>
+        <v>246</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="18"/>
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" s="15"/>
       <c r="C60" s="5" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>180</v>
+        <v>185</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="G60" s="7">
+        <v>45678</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="18"/>
-      <c r="C61" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G61" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="18"/>
-      <c r="C62" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G62" s="7">
-        <v>45678</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="18"/>
-      <c r="C63" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="D63" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="G63" s="7">
-        <v>45678</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>194</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="B46:B51"/>
+    <mergeCell ref="B36:B42"/>
+    <mergeCell ref="B43:B48"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="B56:B60"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="B49:B55"/>
     <mergeCell ref="B7:B10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>